<commit_message>
Eliminadas referencias al schedule de los empleados
</commit_message>
<xml_diff>
--- a/Concept-0/employees.xlsx
+++ b/Concept-0/employees.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bb54ded66f80c8e/UC3M/Cuarto Curso/Trabajo de Fin de Grado/Concept 0/Concept-0/Concept-0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7FB4B4F2-547B-44C4-921D-57385E63BD39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C857EA77-BA40-4EFF-BBAF-5088BDD55858}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{7FB4B4F2-547B-44C4-921D-57385E63BD39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6C0B4F40-92A1-4810-855D-872C939EDB04}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
     <sheet name="Tasks" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Hoja1!$A$1:$C$4</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Hoja1!$A$1:$B$4</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name,Role,Schedule</t>
   </si>
@@ -52,16 +52,10 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Schedule</t>
-  </si>
-  <si>
     <t>Rodrigo</t>
   </si>
   <si>
     <t>CEO</t>
-  </si>
-  <si>
-    <t>9:00-17:00|9:00-15:00</t>
   </si>
   <si>
     <t>Arturo</t>
@@ -605,10 +599,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -631,22 +622,23 @@
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+    <queryTableFields count="2">
       <queryTableField id="1" name="Name" tableColumnId="1"/>
       <queryTableField id="2" name="Role" tableColumnId="2"/>
-      <queryTableField id="3" name="Schedule" tableColumnId="3"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="Schedule"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Employees" displayName="Employees" ref="A1:C4" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Role" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Schedule" queryTableFieldId="3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Employees" displayName="Employees" ref="A1:B4" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Role" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,61 +941,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1023,24 +1003,24 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>